<commit_message>
Started Looking at Alternate Solutions
</commit_message>
<xml_diff>
--- a/CH-048 Transformation.xlsx
+++ b/CH-048 Transformation.xlsx
@@ -1,24 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E862D7-44EE-46C1-9848-02B8A452661F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{A3E24027-88E8-42B4-B0B4-486B39F25AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27C0D9DD-FA62-4E43-B5C1-12AB76A17290}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="My_EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="OutsideReview" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_a">OutsideReview!$B$2:$B$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">My_EDA!$B$1:$B$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$1:$B$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">OutsideReview!$B$1:$B$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -63,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="28">
   <si>
     <t>FA+HS</t>
   </si>
@@ -145,22 +148,25 @@
   <si>
     <t>so</t>
   </si>
+  <si>
+    <t>This is a wonderful solution.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Rockwell"/>
+      <name val="Consolas"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Rockwell"/>
+      <name val="Consolas"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -174,9 +180,16 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Rockwell"/>
+      <name val="Consolas"/>
       <family val="1"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Mono"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -328,10 +341,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -399,8 +413,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -444,8 +460,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3044446" y="2372994"/>
-          <a:ext cx="5787132" cy="2267585"/>
+          <a:off x="3044446" y="2355849"/>
+          <a:ext cx="5794752" cy="2216150"/>
           <a:chOff x="4119814" y="1849363"/>
           <a:chExt cx="4569974" cy="2393950"/>
         </a:xfrm>
@@ -770,10 +786,76 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4B1115F-1A4A-4D31-1A6D-52818272F2CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8298180" y="6492240"/>
+          <a:ext cx="6652260" cy="3802380"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Damask">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Mark-Standard">
   <a:themeElements>
-    <a:clrScheme name="Damask">
+    <a:clrScheme name="Yellow Orange">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -781,175 +863,85 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="2A5B7F"/>
+        <a:srgbClr val="4E3B30"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="ABDAFC"/>
+        <a:srgbClr val="FBEEC9"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="9EC544"/>
+        <a:srgbClr val="F0A22E"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="50BEA3"/>
+        <a:srgbClr val="A5644E"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="4A9CCC"/>
+        <a:srgbClr val="B58B80"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="9A66CA"/>
+        <a:srgbClr val="C3986D"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="C54F71"/>
+        <a:srgbClr val="A19574"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="DE9C3C"/>
+        <a:srgbClr val="C17529"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="6BA9DA"/>
+        <a:srgbClr val="AD1F1F"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="A0BCD3"/>
+        <a:srgbClr val="FFC42F"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Damask">
+    <a:fontScheme name="Biegert Standard">
       <a:majorFont>
-        <a:latin typeface="Bookman Old Style" panose="02050604050505020204"/>
+        <a:latin typeface="Consolas"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Rockwell" panose="02060603020205020403"/>
+        <a:latin typeface="Consolas"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Damask">
+    <a:fmtScheme name="Riblet">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="48000"/>
-                <a:satMod val="105000"/>
-                <a:lumMod val="110000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="78000"/>
-                <a:satMod val="109000"/>
-                <a:lumMod val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="94000"/>
-                <a:satMod val="100000"/>
-                <a:lumMod val="104000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="69000">
-              <a:schemeClr val="phClr">
-                <a:shade val="86000"/>
-                <a:satMod val="130000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="72000"/>
-                <a:satMod val="130000"/>
-                <a:lumMod val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="80000"/>
+            <a:satMod val="150000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="17145" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="58420" cap="flat" cmpd="thickThin" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="phClr"/>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:alpha val="50000"/>
+              <a:satMod val="150000"/>
+            </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -960,18 +952,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="50800" dist="38100" dir="5400000" sy="96000" rotWithShape="0">
+            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="54000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="76200" dist="38100" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="76000"/>
+                <a:alpha val="60000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -979,10 +962,28 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="balanced" dir="t"/>
+            <a:lightRig rig="flat" dir="tl"/>
           </a:scene3d>
-          <a:sp3d prstMaterial="matte">
-            <a:bevelT w="25400" h="25400" prst="relaxedInset"/>
+          <a:sp3d prstMaterial="flat">
+            <a:bevelT w="31750" h="63500" prst="riblet"/>
+          </a:sp3d>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="60000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="flat" dir="tl"/>
+          </a:scene3d>
+          <a:sp3d prstMaterial="flat">
+            <a:bevelT w="57150" h="114300" prst="riblet"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -996,23 +997,33 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:blipFill rotWithShape="1">
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-            <a:duotone>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="18000"/>
-                <a:satMod val="160000"/>
-                <a:lumMod val="28000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="95000"/>
-                <a:satMod val="160000"/>
-                <a:lumMod val="116000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
-            </a:duotone>
-          </a:blip>
-          <a:stretch/>
-        </a:blipFill>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
@@ -1020,7 +1031,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Damask" id="{F9A299A0-33D0-4E0F-9F3F-7163E3744208}" vid="{746EEEEA-FB6A-406B-B510-531588D54811}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1034,7 +1045,7 @@
       <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
     <col min="2" max="2" width="31.8984375" customWidth="1"/>
@@ -1042,7 +1053,7 @@
     <col min="6" max="15" width="4.09765625" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="6" t="s">
         <v>20</v>
       </c>
@@ -1060,7 +1071,7 @@
       <c r="N1" s="24"/>
       <c r="O1" s="24"/>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="8" t="s">
         <v>19</v>
@@ -1097,7 +1108,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="8" t="s">
         <v>1</v>
@@ -1127,7 +1138,7 @@
       </c>
       <c r="O3" s="14"/>
     </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="7" t="s">
         <v>14</v>
@@ -1155,7 +1166,7 @@
       <c r="N4" s="13"/>
       <c r="O4" s="14"/>
     </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="8" t="s">
         <v>18</v>
@@ -1177,7 +1188,7 @@
       <c r="N5" s="13"/>
       <c r="O5" s="14"/>
     </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="20" t="s">
         <v>0</v>
@@ -1198,7 +1209,7 @@
       <c r="N6" s="13"/>
       <c r="O6" s="14"/>
     </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="7" t="s">
         <v>1</v>
@@ -1226,7 +1237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="7" t="s">
         <v>2</v>
@@ -1247,7 +1258,7 @@
       <c r="N8" s="13"/>
       <c r="O8" s="14"/>
     </row>
-    <row r="9" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="7" t="s">
         <v>16</v>
@@ -1276,7 +1287,7 @@
       </c>
       <c r="O9" s="16"/>
     </row>
-    <row r="10" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="8" t="s">
         <v>3</v>
@@ -1298,7 +1309,7 @@
       <c r="N10" s="15"/>
       <c r="O10" s="16"/>
     </row>
-    <row r="11" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="22" t="s">
         <v>21</v>
@@ -1322,7 +1333,7 @@
       <c r="N11" s="15"/>
       <c r="O11" s="16"/>
     </row>
-    <row r="12" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
@@ -1345,7 +1356,7 @@
       <c r="N12" s="15"/>
       <c r="O12" s="16"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="8" t="s">
         <v>4</v>
@@ -1363,21 +1374,21 @@
       <c r="N13"/>
       <c r="O13"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="8" t="s">
         <v>22</v>
@@ -1385,7 +1396,7 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="8" t="s">
         <v>5</v>
@@ -1393,21 +1404,21 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="23" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="8" t="s">
         <v>25</v>
@@ -1418,21 +1429,21 @@
       <c r="G20" s="18"/>
       <c r="H20" s="18"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C21" s="1"/>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
       <c r="H21" s="18"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C22" s="1"/>
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
       <c r="G22" s="18"/>
       <c r="H22" s="18"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1441,7 +1452,7 @@
       <c r="G23" s="18"/>
       <c r="H23" s="18"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="C24" s="1"/>
       <c r="E24" s="18"/>
@@ -1449,7 +1460,7 @@
       <c r="G24" s="18"/>
       <c r="H24" s="18"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="1"/>
       <c r="E25" s="18"/>
@@ -1457,7 +1468,7 @@
       <c r="G25" s="18"/>
       <c r="H25" s="18"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
       <c r="C26" s="1"/>
       <c r="E26" s="18"/>
@@ -1465,73 +1476,73 @@
       <c r="G26" s="18"/>
       <c r="H26" s="18"/>
     </row>
-    <row r="27" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="18"/>
       <c r="H27" s="18"/>
     </row>
-    <row r="28" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="18"/>
       <c r="H28" s="18"/>
     </row>
-    <row r="29" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
       <c r="G29" s="18"/>
       <c r="H29" s="18"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
       <c r="G30" s="18"/>
       <c r="H30" s="18"/>
     </row>
-    <row r="31" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
       <c r="G31" s="18"/>
       <c r="H31" s="18"/>
     </row>
-    <row r="32" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
       <c r="G32" s="18"/>
       <c r="H32" s="18"/>
     </row>
-    <row r="33" spans="5:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
       <c r="G33" s="18"/>
       <c r="H33" s="18"/>
     </row>
-    <row r="34" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E34" s="18"/>
       <c r="F34" s="18"/>
       <c r="G34" s="18"/>
       <c r="H34" s="18"/>
     </row>
-    <row r="35" spans="5:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
       <c r="G35" s="18"/>
       <c r="H35" s="18"/>
     </row>
-    <row r="36" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
       <c r="G36" s="18"/>
       <c r="H36" s="18"/>
     </row>
-    <row r="37" spans="5:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E37" s="18"/>
       <c r="F37" s="18"/>
       <c r="G37" s="18"/>
       <c r="H37" s="18"/>
     </row>
-    <row r="38" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
       <c r="G38" s="18"/>
@@ -1555,11 +1566,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988169DE-4857-4A00-8A4B-45951DE2D3C8}">
   <dimension ref="A1:AA39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
     <col min="2" max="2" width="31.8984375" customWidth="1"/>
@@ -1567,7 +1578,7 @@
     <col min="6" max="15" width="4.09765625" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="6" t="s">
         <v>20</v>
       </c>
@@ -1585,7 +1596,7 @@
       <c r="N1" s="24"/>
       <c r="O1" s="24"/>
     </row>
-    <row r="2" spans="1:27" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="8" t="s">
         <v>19</v>
@@ -1622,7 +1633,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:27" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="8" t="s">
         <v>1</v>
@@ -1683,7 +1694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:27" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="7" t="s">
         <v>14</v>
@@ -1741,7 +1752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:27" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="8" t="s">
         <v>18</v>
@@ -1793,7 +1804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:27" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="20" t="s">
         <v>0</v>
@@ -1844,7 +1855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:27" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="7" t="s">
         <v>1</v>
@@ -1902,7 +1913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:27" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="7" t="s">
         <v>2</v>
@@ -1953,7 +1964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="7" t="s">
         <v>16</v>
@@ -2012,7 +2023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="8" t="s">
         <v>3</v>
@@ -2064,7 +2075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="22" t="s">
         <v>21</v>
@@ -2118,7 +2129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
@@ -2171,7 +2182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="8" t="s">
         <v>4</v>
@@ -2189,21 +2200,21 @@
       <c r="N13"/>
       <c r="O13"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="8" t="s">
         <v>22</v>
@@ -2211,7 +2222,7 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="8" t="s">
         <v>5</v>
@@ -2219,21 +2230,21 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="23" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="8" t="s">
         <v>25</v>
@@ -2244,7 +2255,7 @@
       <c r="G20" s="18"/>
       <c r="H20" s="18"/>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C21" s="1"/>
       <c r="E21" s="18" t="str" cm="1">
         <f t="array" ref="E21:N21">TRANSPOSE(_xlfn.ANCHORARRAY(D22))</f>
@@ -2285,7 +2296,7 @@
         <v>CS</v>
       </c>
       <c r="S21" t="str">
-        <f>Q21&amp;R21</f>
+        <f t="shared" ref="S21:S39" si="0">Q21&amp;R21</f>
         <v>GACS</v>
       </c>
       <c r="W21" t="str" cm="1">
@@ -2308,7 +2319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C22" s="1"/>
       <c r="D22" t="str" cm="1">
         <f t="array" ref="D22:D31">_xlfn.LET(_xlpm.x,_xlfn.DROP(_xlfn.UNIQUE(_xlfn.TOCOL(_xlfn.REDUCE("",B2:B20,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TEXTSPLIT(_xlpm.v,"+")))),3)),1),_xlfn.SORTBY(_xlpm.x,_xlfn.XMATCH(_xlpm.x,E3:E12),1))</f>
@@ -2361,7 +2372,7 @@
         <v>PSO</v>
       </c>
       <c r="S22" t="str">
-        <f>Q22&amp;R22</f>
+        <f t="shared" si="0"/>
         <v>GAPSO</v>
       </c>
       <c r="W22" t="str">
@@ -2371,18 +2382,18 @@
         <v>PSO</v>
       </c>
       <c r="Y22" t="str">
-        <f t="shared" ref="Y22:Y35" si="0">W22&amp;X22</f>
+        <f t="shared" ref="Y22:Y35" si="1">W22&amp;X22</f>
         <v>GAPSO</v>
       </c>
       <c r="Z22" t="str">
-        <f t="shared" ref="Z22:Z35" si="1">X22&amp;W22</f>
+        <f t="shared" ref="Z22:Z35" si="2">X22&amp;W22</f>
         <v>PSOGA</v>
       </c>
       <c r="AA22">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="str">
@@ -2435,7 +2446,7 @@
         <v>GA</v>
       </c>
       <c r="S23" t="str">
-        <f>Q23&amp;R23</f>
+        <f t="shared" si="0"/>
         <v>PSOGA</v>
       </c>
       <c r="W23" t="str">
@@ -2445,18 +2456,18 @@
         <v>GA</v>
       </c>
       <c r="Y23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>PSOGA</v>
       </c>
       <c r="Z23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GAPSO</v>
       </c>
       <c r="AA23">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="C24" s="1"/>
       <c r="D24" t="str">
@@ -2509,7 +2520,7 @@
         <v>PSO</v>
       </c>
       <c r="S24" t="str">
-        <f>Q24&amp;R24</f>
+        <f t="shared" si="0"/>
         <v>DEPSO</v>
       </c>
       <c r="W24" t="str">
@@ -2519,18 +2530,18 @@
         <v>PSO</v>
       </c>
       <c r="Y24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>DEPSO</v>
       </c>
       <c r="Z24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>PSODE</v>
       </c>
       <c r="AA24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="1"/>
       <c r="D25" t="str">
@@ -2583,7 +2594,7 @@
         <v>HS</v>
       </c>
       <c r="S25" t="str">
-        <f>Q25&amp;R25</f>
+        <f t="shared" si="0"/>
         <v>FAHS</v>
       </c>
       <c r="W25" t="str">
@@ -2593,18 +2604,18 @@
         <v>HS</v>
       </c>
       <c r="Y25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>FAHS</v>
       </c>
       <c r="Z25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HSFA</v>
       </c>
       <c r="AA25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
       <c r="C26" s="1"/>
       <c r="D26" t="str">
@@ -2657,7 +2668,7 @@
         <v>PSO</v>
       </c>
       <c r="S26" t="str">
-        <f>Q26&amp;R26</f>
+        <f t="shared" si="0"/>
         <v>GAPSO</v>
       </c>
       <c r="W26" t="str">
@@ -2667,71 +2678,71 @@
         <v>TS</v>
       </c>
       <c r="Y26" t="str">
+        <f t="shared" si="1"/>
+        <v>GATS</v>
+      </c>
+      <c r="Z26" t="str">
+        <f t="shared" si="2"/>
+        <v>TSGA</v>
+      </c>
+      <c r="AA26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D27" t="str">
+        <v>RO</v>
+      </c>
+      <c r="E27" s="18" cm="1">
+        <f t="array" ref="E27">_xlfn.XLOOKUP($D27&amp;E$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="F27" s="18" t="str" cm="1">
+        <f t="array" ref="F27">_xlfn.XLOOKUP($D27&amp;F$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="G27" s="18" t="str" cm="1">
+        <f t="array" ref="G27">_xlfn.XLOOKUP($D27&amp;G$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="H27" s="18" t="str" cm="1">
+        <f t="array" ref="H27">_xlfn.XLOOKUP($D27&amp;H$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="I27" s="18" t="str" cm="1">
+        <f t="array" ref="I27">_xlfn.XLOOKUP($D27&amp;I$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="J27" s="18" t="str" cm="1">
+        <f t="array" ref="J27">_xlfn.XLOOKUP($D27&amp;J$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="K27" s="18" t="str" cm="1">
+        <f t="array" ref="K27">_xlfn.XLOOKUP($D27&amp;K$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="L27" s="18" t="str" cm="1">
+        <f t="array" ref="L27">_xlfn.XLOOKUP($D27&amp;L$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="M27" s="18" t="str" cm="1">
+        <f t="array" ref="M27">_xlfn.XLOOKUP($D27&amp;M$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="N27" s="18" t="str" cm="1">
+        <f t="array" ref="N27">_xlfn.XLOOKUP($D27&amp;N$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="Q27" t="str">
+        <v>GA</v>
+      </c>
+      <c r="R27" t="str">
+        <v>TS</v>
+      </c>
+      <c r="S27" t="str">
         <f t="shared" si="0"/>
         <v>GATS</v>
       </c>
-      <c r="Z26" t="str">
-        <f t="shared" si="1"/>
-        <v>TSGA</v>
-      </c>
-      <c r="AA26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D27" t="str">
-        <v>RO</v>
-      </c>
-      <c r="E27" s="18" cm="1">
-        <f t="array" ref="E27">_xlfn.XLOOKUP($D27&amp;E$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v>1</v>
-      </c>
-      <c r="F27" s="18" t="str" cm="1">
-        <f t="array" ref="F27">_xlfn.XLOOKUP($D27&amp;F$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="G27" s="18" t="str" cm="1">
-        <f t="array" ref="G27">_xlfn.XLOOKUP($D27&amp;G$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="H27" s="18" t="str" cm="1">
-        <f t="array" ref="H27">_xlfn.XLOOKUP($D27&amp;H$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="I27" s="18" t="str" cm="1">
-        <f t="array" ref="I27">_xlfn.XLOOKUP($D27&amp;I$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="J27" s="18" t="str" cm="1">
-        <f t="array" ref="J27">_xlfn.XLOOKUP($D27&amp;J$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="K27" s="18" t="str" cm="1">
-        <f t="array" ref="K27">_xlfn.XLOOKUP($D27&amp;K$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="L27" s="18" t="str" cm="1">
-        <f t="array" ref="L27">_xlfn.XLOOKUP($D27&amp;L$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="M27" s="18" t="str" cm="1">
-        <f t="array" ref="M27">_xlfn.XLOOKUP($D27&amp;M$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="N27" s="18" t="str" cm="1">
-        <f t="array" ref="N27">_xlfn.XLOOKUP($D27&amp;N$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="Q27" t="str">
-        <v>GA</v>
-      </c>
-      <c r="R27" t="str">
-        <v>TS</v>
-      </c>
-      <c r="S27" t="str">
-        <f>Q27&amp;R27</f>
-        <v>GATS</v>
-      </c>
       <c r="W27" t="str">
         <v>HS</v>
       </c>
@@ -2739,18 +2750,18 @@
         <v>MPSO</v>
       </c>
       <c r="Y27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>HSMPSO</v>
       </c>
       <c r="Z27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>MPSOHS</v>
       </c>
       <c r="AA27">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D28" t="str">
         <v>SO</v>
       </c>
@@ -2801,7 +2812,7 @@
         <v>MPSO</v>
       </c>
       <c r="S28" t="str">
-        <f>Q28&amp;R28</f>
+        <f t="shared" si="0"/>
         <v>HSMPSO</v>
       </c>
       <c r="W28" t="str">
@@ -2811,162 +2822,162 @@
         <v>PSO</v>
       </c>
       <c r="Y28" t="str">
+        <f t="shared" si="1"/>
+        <v>HSPSO</v>
+      </c>
+      <c r="Z28" t="str">
+        <f t="shared" si="2"/>
+        <v>PSOHS</v>
+      </c>
+      <c r="AA28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D29" t="str">
+        <v>CS</v>
+      </c>
+      <c r="E29" s="18" cm="1">
+        <f t="array" ref="E29">_xlfn.XLOOKUP($D29&amp;E$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="F29" s="18" t="str" cm="1">
+        <f t="array" ref="F29">_xlfn.XLOOKUP($D29&amp;F$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="G29" s="18" t="str" cm="1">
+        <f t="array" ref="G29">_xlfn.XLOOKUP($D29&amp;G$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="H29" s="18" t="str" cm="1">
+        <f t="array" ref="H29">_xlfn.XLOOKUP($D29&amp;H$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="I29" s="18" t="str" cm="1">
+        <f t="array" ref="I29">_xlfn.XLOOKUP($D29&amp;I$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="J29" s="18" t="str" cm="1">
+        <f t="array" ref="J29">_xlfn.XLOOKUP($D29&amp;J$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="K29" s="18" t="str" cm="1">
+        <f t="array" ref="K29">_xlfn.XLOOKUP($D29&amp;K$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="L29" s="18" t="str" cm="1">
+        <f t="array" ref="L29">_xlfn.XLOOKUP($D29&amp;L$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="M29" s="18" t="str" cm="1">
+        <f t="array" ref="M29">_xlfn.XLOOKUP($D29&amp;M$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="N29" s="18" t="str" cm="1">
+        <f t="array" ref="N29">_xlfn.XLOOKUP($D29&amp;N$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="Q29" t="str">
+        <v>HS</v>
+      </c>
+      <c r="R29" t="str">
+        <v>PSO</v>
+      </c>
+      <c r="S29" t="str">
         <f t="shared" si="0"/>
         <v>HSPSO</v>
       </c>
-      <c r="Z28" t="str">
+      <c r="W29" t="str">
+        <v>HS</v>
+      </c>
+      <c r="X29" t="str">
+        <v>SO</v>
+      </c>
+      <c r="Y29" t="str">
+        <f t="shared" si="1"/>
+        <v>HSSO</v>
+      </c>
+      <c r="Z29" t="str">
+        <f t="shared" si="2"/>
+        <v>SOHS</v>
+      </c>
+      <c r="AA29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="D30" t="str">
+        <v>TS</v>
+      </c>
+      <c r="E30" s="18" cm="1">
+        <f t="array" ref="E30">_xlfn.XLOOKUP($D30&amp;E$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="F30" s="18" t="str" cm="1">
+        <f t="array" ref="F30">_xlfn.XLOOKUP($D30&amp;F$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="G30" s="18" t="str" cm="1">
+        <f t="array" ref="G30">_xlfn.XLOOKUP($D30&amp;G$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="H30" s="18" t="str" cm="1">
+        <f t="array" ref="H30">_xlfn.XLOOKUP($D30&amp;H$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="I30" s="18" t="str" cm="1">
+        <f t="array" ref="I30">_xlfn.XLOOKUP($D30&amp;I$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="J30" s="18" t="str" cm="1">
+        <f t="array" ref="J30">_xlfn.XLOOKUP($D30&amp;J$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="K30" s="18" cm="1">
+        <f t="array" ref="K30">_xlfn.XLOOKUP($D30&amp;K$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="L30" s="18" t="str" cm="1">
+        <f t="array" ref="L30">_xlfn.XLOOKUP($D30&amp;L$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="M30" s="18" t="str" cm="1">
+        <f t="array" ref="M30">_xlfn.XLOOKUP($D30&amp;M$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="N30" s="18" t="str" cm="1">
+        <f t="array" ref="N30">_xlfn.XLOOKUP($D30&amp;N$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
+        <v/>
+      </c>
+      <c r="Q30" t="str">
+        <v>HS</v>
+      </c>
+      <c r="R30" t="str">
+        <v>SO</v>
+      </c>
+      <c r="S30" t="str">
+        <f t="shared" si="0"/>
+        <v>HSSO</v>
+      </c>
+      <c r="W30" t="str">
+        <v>PSO</v>
+      </c>
+      <c r="X30" t="str">
+        <v>HS</v>
+      </c>
+      <c r="Y30" t="str">
         <f t="shared" si="1"/>
         <v>PSOHS</v>
       </c>
-      <c r="AA28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" t="str">
-        <v>CS</v>
-      </c>
-      <c r="E29" s="18" cm="1">
-        <f t="array" ref="E29">_xlfn.XLOOKUP($D29&amp;E$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v>1</v>
-      </c>
-      <c r="F29" s="18" t="str" cm="1">
-        <f t="array" ref="F29">_xlfn.XLOOKUP($D29&amp;F$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="G29" s="18" t="str" cm="1">
-        <f t="array" ref="G29">_xlfn.XLOOKUP($D29&amp;G$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="H29" s="18" t="str" cm="1">
-        <f t="array" ref="H29">_xlfn.XLOOKUP($D29&amp;H$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="I29" s="18" t="str" cm="1">
-        <f t="array" ref="I29">_xlfn.XLOOKUP($D29&amp;I$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="J29" s="18" t="str" cm="1">
-        <f t="array" ref="J29">_xlfn.XLOOKUP($D29&amp;J$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="K29" s="18" t="str" cm="1">
-        <f t="array" ref="K29">_xlfn.XLOOKUP($D29&amp;K$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="L29" s="18" t="str" cm="1">
-        <f t="array" ref="L29">_xlfn.XLOOKUP($D29&amp;L$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="M29" s="18" t="str" cm="1">
-        <f t="array" ref="M29">_xlfn.XLOOKUP($D29&amp;M$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="N29" s="18" t="str" cm="1">
-        <f t="array" ref="N29">_xlfn.XLOOKUP($D29&amp;N$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="Q29" t="str">
-        <v>HS</v>
-      </c>
-      <c r="R29" t="str">
-        <v>PSO</v>
-      </c>
-      <c r="S29" t="str">
-        <f>Q29&amp;R29</f>
-        <v>HSPSO</v>
-      </c>
-      <c r="W29" t="str">
-        <v>HS</v>
-      </c>
-      <c r="X29" t="str">
-        <v>SO</v>
-      </c>
-      <c r="Y29" t="str">
-        <f t="shared" si="0"/>
-        <v>HSSO</v>
-      </c>
-      <c r="Z29" t="str">
-        <f t="shared" si="1"/>
-        <v>SOHS</v>
-      </c>
-      <c r="AA29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="D30" t="str">
-        <v>TS</v>
-      </c>
-      <c r="E30" s="18" cm="1">
-        <f t="array" ref="E30">_xlfn.XLOOKUP($D30&amp;E$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v>1</v>
-      </c>
-      <c r="F30" s="18" t="str" cm="1">
-        <f t="array" ref="F30">_xlfn.XLOOKUP($D30&amp;F$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="G30" s="18" t="str" cm="1">
-        <f t="array" ref="G30">_xlfn.XLOOKUP($D30&amp;G$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="H30" s="18" t="str" cm="1">
-        <f t="array" ref="H30">_xlfn.XLOOKUP($D30&amp;H$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="I30" s="18" t="str" cm="1">
-        <f t="array" ref="I30">_xlfn.XLOOKUP($D30&amp;I$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="J30" s="18" t="str" cm="1">
-        <f t="array" ref="J30">_xlfn.XLOOKUP($D30&amp;J$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="K30" s="18" cm="1">
-        <f t="array" ref="K30">_xlfn.XLOOKUP($D30&amp;K$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v>1</v>
-      </c>
-      <c r="L30" s="18" t="str" cm="1">
-        <f t="array" ref="L30">_xlfn.XLOOKUP($D30&amp;L$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="M30" s="18" t="str" cm="1">
-        <f t="array" ref="M30">_xlfn.XLOOKUP($D30&amp;M$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="N30" s="18" t="str" cm="1">
-        <f t="array" ref="N30">_xlfn.XLOOKUP($D30&amp;N$21,_xlfn.VSTACK($Y$21:$Y$35,$Z$21:$Z$35),_xlfn.VSTACK($AA$21:$AA$35,_xlfn.ANCHORARRAY($AA$21)),"")</f>
-        <v/>
-      </c>
-      <c r="Q30" t="str">
-        <v>HS</v>
-      </c>
-      <c r="R30" t="str">
-        <v>SO</v>
-      </c>
-      <c r="S30" t="str">
-        <f>Q30&amp;R30</f>
-        <v>HSSO</v>
-      </c>
-      <c r="W30" t="str">
-        <v>PSO</v>
-      </c>
-      <c r="X30" t="str">
-        <v>HS</v>
-      </c>
-      <c r="Y30" t="str">
-        <f t="shared" si="0"/>
-        <v>PSOHS</v>
-      </c>
       <c r="Z30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HSPSO</v>
       </c>
       <c r="AA30">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D31" t="str">
         <v>MPSO</v>
       </c>
@@ -3017,7 +3028,7 @@
         <v>GA</v>
       </c>
       <c r="S31" t="str">
-        <f>Q31&amp;R31</f>
+        <f t="shared" si="0"/>
         <v>PSOGA</v>
       </c>
       <c r="W31" t="str">
@@ -3027,18 +3038,18 @@
         <v>SO</v>
       </c>
       <c r="Y31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>PSOSO</v>
       </c>
       <c r="Z31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>SOPSO</v>
       </c>
       <c r="AA31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
       <c r="G32" s="18"/>
@@ -3050,7 +3061,7 @@
         <v>HS</v>
       </c>
       <c r="S32" t="str">
-        <f>Q32&amp;R32</f>
+        <f t="shared" si="0"/>
         <v>PSOHS</v>
       </c>
       <c r="W32" t="str">
@@ -3060,18 +3071,18 @@
         <v>GA</v>
       </c>
       <c r="Y32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ROGA</v>
       </c>
       <c r="Z32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GARO</v>
       </c>
       <c r="AA32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="5:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
       <c r="G33" s="18"/>
@@ -3083,7 +3094,7 @@
         <v>GA</v>
       </c>
       <c r="S33" t="str">
-        <f>Q33&amp;R33</f>
+        <f t="shared" si="0"/>
         <v>PSOGA</v>
       </c>
       <c r="W33" t="str">
@@ -3093,18 +3104,18 @@
         <v>GA</v>
       </c>
       <c r="Y33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>SOGA</v>
       </c>
       <c r="Z33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GASO</v>
       </c>
       <c r="AA33">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:27" x14ac:dyDescent="0.3">
       <c r="E34" s="18"/>
       <c r="F34" s="18"/>
       <c r="G34" s="18"/>
@@ -3116,7 +3127,7 @@
         <v>GA</v>
       </c>
       <c r="S34" t="str">
-        <f>Q34&amp;R34</f>
+        <f t="shared" si="0"/>
         <v>PSOGA</v>
       </c>
       <c r="W34" t="str">
@@ -3126,18 +3137,18 @@
         <v>HS</v>
       </c>
       <c r="Y34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>SOHS</v>
       </c>
       <c r="Z34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HSSO</v>
       </c>
       <c r="AA34">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="5:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
       <c r="G35" s="18"/>
@@ -3149,7 +3160,7 @@
         <v>SO</v>
       </c>
       <c r="S35" t="str">
-        <f>Q35&amp;R35</f>
+        <f t="shared" si="0"/>
         <v>PSOSO</v>
       </c>
       <c r="W35" t="str">
@@ -3159,18 +3170,18 @@
         <v>TS</v>
       </c>
       <c r="Y35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>SOTS</v>
       </c>
       <c r="Z35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>TSSO</v>
       </c>
       <c r="AA35">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:27" x14ac:dyDescent="0.3">
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
       <c r="G36" s="18"/>
@@ -3182,11 +3193,11 @@
         <v>GA</v>
       </c>
       <c r="S36" t="str">
-        <f>Q36&amp;R36</f>
+        <f t="shared" si="0"/>
         <v>ROGA</v>
       </c>
     </row>
-    <row r="37" spans="5:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E37" s="18"/>
       <c r="F37" s="18"/>
       <c r="G37" s="18"/>
@@ -3198,11 +3209,11 @@
         <v>GA</v>
       </c>
       <c r="S37" t="str">
-        <f>Q37&amp;R37</f>
+        <f t="shared" si="0"/>
         <v>SOGA</v>
       </c>
     </row>
-    <row r="38" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:27" x14ac:dyDescent="0.3">
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
       <c r="G38" s="18"/>
@@ -3214,11 +3225,11 @@
         <v>HS</v>
       </c>
       <c r="S38" t="str">
-        <f>Q38&amp;R38</f>
+        <f t="shared" si="0"/>
         <v>SOHS</v>
       </c>
     </row>
-    <row r="39" spans="5:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:27" x14ac:dyDescent="0.3">
       <c r="Q39" t="str">
         <v>SO</v>
       </c>
@@ -3226,7 +3237,7 @@
         <v>TS</v>
       </c>
       <c r="S39" t="str">
-        <f>Q39&amp;R39</f>
+        <f t="shared" si="0"/>
         <v>SOTS</v>
       </c>
     </row>
@@ -3237,4 +3248,2070 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0D5CD49-37CF-4261-80F1-294A533B089A}">
+  <dimension ref="A1:AA93"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U13" sqref="U13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="2" max="2" width="31.8984375" customWidth="1"/>
+    <col min="5" max="5" width="5.09765625" style="17" customWidth="1"/>
+    <col min="6" max="15" width="4.09765625" style="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+    </row>
+    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13">
+        <v>6</v>
+      </c>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13">
+        <v>1</v>
+      </c>
+      <c r="L3" s="13">
+        <v>1</v>
+      </c>
+      <c r="M3" s="13">
+        <v>1</v>
+      </c>
+      <c r="N3" s="13">
+        <v>1</v>
+      </c>
+      <c r="O3" s="14"/>
+    </row>
+    <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4"/>
+      <c r="E4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="13">
+        <v>6</v>
+      </c>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13">
+        <v>1</v>
+      </c>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13">
+        <v>2</v>
+      </c>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13">
+        <v>1</v>
+      </c>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="14"/>
+    </row>
+    <row r="5" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5"/>
+      <c r="E5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13">
+        <v>1</v>
+      </c>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="14"/>
+    </row>
+    <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13">
+        <v>1</v>
+      </c>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="14"/>
+    </row>
+    <row r="7" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7"/>
+      <c r="E7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13">
+        <v>2</v>
+      </c>
+      <c r="H7" s="13"/>
+      <c r="I7" s="19">
+        <v>1</v>
+      </c>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13">
+        <v>2</v>
+      </c>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="13">
+        <v>1</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="14"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="15">
+        <v>1</v>
+      </c>
+      <c r="G9" s="15">
+        <v>1</v>
+      </c>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="21">
+        <v>2</v>
+      </c>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15">
+        <v>1</v>
+      </c>
+      <c r="O9" s="16"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="5"/>
+      <c r="B10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="E10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="15">
+        <v>1</v>
+      </c>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="16"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+      <c r="B11" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="E11" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="15">
+        <v>1</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15">
+        <v>1</v>
+      </c>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="16"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15">
+        <v>1</v>
+      </c>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="16"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+      <c r="B13" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
+      <c r="B19" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="C21" s="1"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="P21" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="C22" s="1"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B23" s="2"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B24" s="2"/>
+      <c r="C24" s="1"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="Q24" t="str" cm="1">
+        <f t="array" ref="Q24:AA34">_xlfn.LET(_xlpm.a,B2:B20,_xlpm.b,_xlfn.UNIQUE(_xlfn.VSTACK(_xlfn.TEXTBEFORE(_xlpm.a,"+"),_xlfn.TEXTAFTER(_xlpm.a,"+"))),_xlpm.c,TRANSPOSE(_xlpm.b),_xlfn.HSTACK(_xlfn.VSTACK("",_xlpm.b),_xlfn.VSTACK(_xlpm.c,_xlfn.MAP(_xlpm.b&amp;"+"&amp;_xlpm.c,_xlpm.c&amp;"+"&amp;_xlpm.b,_xlfn.LAMBDA(_xlpm.x,_xlpm.y,SUM((_xlpm.a=_xlpm.x)+(_xlpm.a=_xlpm.y)))))))</f>
+        <v/>
+      </c>
+      <c r="R24" t="str">
+        <v>GA</v>
+      </c>
+      <c r="S24" t="str">
+        <v>PSO</v>
+      </c>
+      <c r="T24" t="str">
+        <v>DE</v>
+      </c>
+      <c r="U24" t="str">
+        <v>FA</v>
+      </c>
+      <c r="V24" t="str">
+        <v>HS</v>
+      </c>
+      <c r="W24" t="str">
+        <v>RO</v>
+      </c>
+      <c r="X24" t="str">
+        <v>SO</v>
+      </c>
+      <c r="Y24" t="str">
+        <v>CS</v>
+      </c>
+      <c r="Z24" t="str">
+        <v>TS</v>
+      </c>
+      <c r="AA24" t="str">
+        <v>MPSO</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B25" s="2"/>
+      <c r="C25" s="1"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="Q25" t="str">
+        <v>GA</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>6</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>1</v>
+      </c>
+      <c r="X25">
+        <v>1</v>
+      </c>
+      <c r="Y25">
+        <v>1</v>
+      </c>
+      <c r="Z25">
+        <v>1</v>
+      </c>
+      <c r="AA25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B26" s="2"/>
+      <c r="C26" s="1"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="Q26" t="str">
+        <v>PSO</v>
+      </c>
+      <c r="R26">
+        <v>6</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>1</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>2</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <v>1</v>
+      </c>
+      <c r="Y26">
+        <v>0</v>
+      </c>
+      <c r="Z26">
+        <v>0</v>
+      </c>
+      <c r="AA26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="Q27" t="str">
+        <v>DE</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>1</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="Q28" t="str">
+        <v>FA</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>1</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <v>0</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
+      <c r="AA28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="Q29" t="str">
+        <v>HS</v>
+      </c>
+      <c r="R29">
+        <v>0</v>
+      </c>
+      <c r="S29">
+        <v>2</v>
+      </c>
+      <c r="T29">
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <v>1</v>
+      </c>
+      <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <v>0</v>
+      </c>
+      <c r="X29">
+        <v>2</v>
+      </c>
+      <c r="Y29">
+        <v>0</v>
+      </c>
+      <c r="Z29">
+        <v>0</v>
+      </c>
+      <c r="AA29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="Q30" t="str">
+        <v>RO</v>
+      </c>
+      <c r="R30">
+        <v>1</v>
+      </c>
+      <c r="S30">
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <v>0</v>
+      </c>
+      <c r="X30">
+        <v>0</v>
+      </c>
+      <c r="Y30">
+        <v>0</v>
+      </c>
+      <c r="Z30">
+        <v>0</v>
+      </c>
+      <c r="AA30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="Q31" t="str">
+        <v>SO</v>
+      </c>
+      <c r="R31">
+        <v>1</v>
+      </c>
+      <c r="S31">
+        <v>1</v>
+      </c>
+      <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <v>0</v>
+      </c>
+      <c r="V31">
+        <v>2</v>
+      </c>
+      <c r="W31">
+        <v>0</v>
+      </c>
+      <c r="X31">
+        <v>0</v>
+      </c>
+      <c r="Y31">
+        <v>0</v>
+      </c>
+      <c r="Z31">
+        <v>1</v>
+      </c>
+      <c r="AA31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="Q32" t="str">
+        <v>CS</v>
+      </c>
+      <c r="R32">
+        <v>1</v>
+      </c>
+      <c r="S32">
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <v>0</v>
+      </c>
+      <c r="X32">
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <v>0</v>
+      </c>
+      <c r="Z32">
+        <v>0</v>
+      </c>
+      <c r="AA32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="3:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="Q33" t="str">
+        <v>TS</v>
+      </c>
+      <c r="R33">
+        <v>1</v>
+      </c>
+      <c r="S33">
+        <v>0</v>
+      </c>
+      <c r="T33">
+        <v>0</v>
+      </c>
+      <c r="U33">
+        <v>0</v>
+      </c>
+      <c r="V33">
+        <v>0</v>
+      </c>
+      <c r="W33">
+        <v>0</v>
+      </c>
+      <c r="X33">
+        <v>1</v>
+      </c>
+      <c r="Y33">
+        <v>0</v>
+      </c>
+      <c r="Z33">
+        <v>0</v>
+      </c>
+      <c r="AA33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="3:27" x14ac:dyDescent="0.3">
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="Q34" t="str">
+        <v>MPSO</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <v>0</v>
+      </c>
+      <c r="T34">
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <v>1</v>
+      </c>
+      <c r="W34">
+        <v>0</v>
+      </c>
+      <c r="X34">
+        <v>0</v>
+      </c>
+      <c r="Y34">
+        <v>0</v>
+      </c>
+      <c r="Z34">
+        <v>0</v>
+      </c>
+      <c r="AA34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="3:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+    </row>
+    <row r="36" spans="3:27" x14ac:dyDescent="0.3">
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+    </row>
+    <row r="37" spans="3:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+    </row>
+    <row r="38" spans="3:27" x14ac:dyDescent="0.3">
+      <c r="E38" s="18"/>
+    </row>
+    <row r="39" spans="3:27" x14ac:dyDescent="0.3">
+      <c r="F39" s="18" t="str" cm="1">
+        <f t="array" ref="F39:O39">TRANSPOSE(_xlfn.ANCHORARRAY(E40))</f>
+        <v>GA</v>
+      </c>
+      <c r="G39" s="18" t="str">
+        <v>PSO</v>
+      </c>
+      <c r="H39" s="18" t="str">
+        <v>DE</v>
+      </c>
+      <c r="I39" s="17" t="str">
+        <v>FA</v>
+      </c>
+      <c r="J39" s="17" t="str">
+        <v>HS</v>
+      </c>
+      <c r="K39" s="17" t="str">
+        <v>RO</v>
+      </c>
+      <c r="L39" s="17" t="str">
+        <v>SO</v>
+      </c>
+      <c r="M39" s="17" t="str">
+        <v>CS</v>
+      </c>
+      <c r="N39" s="17" t="str">
+        <v>TS</v>
+      </c>
+      <c r="O39" s="17" t="str">
+        <v>MPSO</v>
+      </c>
+    </row>
+    <row r="40" spans="3:27" x14ac:dyDescent="0.3">
+      <c r="C40" t="str" cm="1">
+        <f t="array" ref="C40:C58">_xlfn.TEXTBEFORE(B2:B20,"+")</f>
+        <v>GA</v>
+      </c>
+      <c r="D40" t="str" cm="1">
+        <f t="array" ref="D40:D58">_xlfn.TEXTAFTER(B2:B20,"+")</f>
+        <v>CS</v>
+      </c>
+      <c r="E40" s="17" t="str" cm="1">
+        <f t="array" ref="E40:E49">_xlfn.UNIQUE(_xlfn.VSTACK(_xlfn.ANCHORARRAY(C40),_xlfn.ANCHORARRAY(D40)))</f>
+        <v>GA</v>
+      </c>
+    </row>
+    <row r="41" spans="3:27" x14ac:dyDescent="0.3">
+      <c r="C41" t="str">
+        <v>GA</v>
+      </c>
+      <c r="D41" t="str">
+        <v>PSO</v>
+      </c>
+      <c r="E41" s="17" t="str">
+        <v>PSO</v>
+      </c>
+    </row>
+    <row r="42" spans="3:27" x14ac:dyDescent="0.3">
+      <c r="C42" t="str">
+        <v>PSO</v>
+      </c>
+      <c r="D42" t="str">
+        <v>GA</v>
+      </c>
+      <c r="E42" s="17" t="str">
+        <v>DE</v>
+      </c>
+    </row>
+    <row r="43" spans="3:27" x14ac:dyDescent="0.3">
+      <c r="C43" t="str">
+        <v>DE</v>
+      </c>
+      <c r="D43" t="str">
+        <v>PSO</v>
+      </c>
+      <c r="E43" s="17" t="str">
+        <v>FA</v>
+      </c>
+    </row>
+    <row r="44" spans="3:27" x14ac:dyDescent="0.3">
+      <c r="C44" t="str">
+        <v>FA</v>
+      </c>
+      <c r="D44" t="str">
+        <v>HS</v>
+      </c>
+      <c r="E44" s="17" t="str">
+        <v>HS</v>
+      </c>
+    </row>
+    <row r="45" spans="3:27" x14ac:dyDescent="0.3">
+      <c r="C45" t="str">
+        <v>GA</v>
+      </c>
+      <c r="D45" t="str">
+        <v>PSO</v>
+      </c>
+      <c r="E45" s="17" t="str">
+        <v>RO</v>
+      </c>
+    </row>
+    <row r="46" spans="3:27" x14ac:dyDescent="0.3">
+      <c r="C46" t="str">
+        <v>GA</v>
+      </c>
+      <c r="D46" t="str">
+        <v>TS</v>
+      </c>
+      <c r="E46" s="17" t="str">
+        <v>SO</v>
+      </c>
+    </row>
+    <row r="47" spans="3:27" x14ac:dyDescent="0.3">
+      <c r="C47" t="str">
+        <v>HS</v>
+      </c>
+      <c r="D47" t="str">
+        <v>MPSO</v>
+      </c>
+      <c r="E47" s="17" t="str">
+        <v>CS</v>
+      </c>
+    </row>
+    <row r="48" spans="3:27" x14ac:dyDescent="0.3">
+      <c r="C48" t="str">
+        <v>HS</v>
+      </c>
+      <c r="D48" t="str">
+        <v>PSO</v>
+      </c>
+      <c r="E48" s="17" t="str">
+        <v>TS</v>
+      </c>
+    </row>
+    <row r="49" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C49" t="str">
+        <v>HS</v>
+      </c>
+      <c r="D49" t="str">
+        <v>SO</v>
+      </c>
+      <c r="E49" s="17" t="str">
+        <v>MPSO</v>
+      </c>
+    </row>
+    <row r="50" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C50" t="str">
+        <v>PSO</v>
+      </c>
+      <c r="D50" t="str">
+        <v>GA</v>
+      </c>
+    </row>
+    <row r="51" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C51" t="str">
+        <v>PSO</v>
+      </c>
+      <c r="D51" t="str">
+        <v>HS</v>
+      </c>
+    </row>
+    <row r="52" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C52" t="str">
+        <v>PSO</v>
+      </c>
+      <c r="D52" t="str">
+        <v>GA</v>
+      </c>
+    </row>
+    <row r="53" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C53" t="str">
+        <v>PSO</v>
+      </c>
+      <c r="D53" t="str">
+        <v>GA</v>
+      </c>
+    </row>
+    <row r="54" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C54" t="str">
+        <v>PSO</v>
+      </c>
+      <c r="D54" t="str">
+        <v>SO</v>
+      </c>
+    </row>
+    <row r="55" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C55" t="str">
+        <v>RO</v>
+      </c>
+      <c r="D55" t="str">
+        <v>GA</v>
+      </c>
+    </row>
+    <row r="56" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C56" t="str">
+        <v>SO</v>
+      </c>
+      <c r="D56" t="str">
+        <v>GA</v>
+      </c>
+    </row>
+    <row r="57" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C57" t="str">
+        <v>SO</v>
+      </c>
+      <c r="D57" t="str">
+        <v>HS</v>
+      </c>
+    </row>
+    <row r="58" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C58" t="str">
+        <v>SO</v>
+      </c>
+      <c r="D58" t="str">
+        <v>TS</v>
+      </c>
+    </row>
+    <row r="60" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="E60" s="17" t="str" cm="1">
+        <f t="array" ref="E60:N69">_xlfn.ANCHORARRAY(E40)&amp;"+"&amp;_xlfn.ANCHORARRAY(F39)</f>
+        <v>GA+GA</v>
+      </c>
+      <c r="F60" s="17" t="str">
+        <v>GA+PSO</v>
+      </c>
+      <c r="G60" s="17" t="str">
+        <v>GA+DE</v>
+      </c>
+      <c r="H60" s="17" t="str">
+        <v>GA+FA</v>
+      </c>
+      <c r="I60" s="17" t="str">
+        <v>GA+HS</v>
+      </c>
+      <c r="J60" s="17" t="str">
+        <v>GA+RO</v>
+      </c>
+      <c r="K60" s="17" t="str">
+        <v>GA+SO</v>
+      </c>
+      <c r="L60" s="17" t="str">
+        <v>GA+CS</v>
+      </c>
+      <c r="M60" s="17" t="str">
+        <v>GA+TS</v>
+      </c>
+      <c r="N60" s="17" t="str">
+        <v>GA+MPSO</v>
+      </c>
+    </row>
+    <row r="61" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="E61" s="17" t="str">
+        <v>PSO+GA</v>
+      </c>
+      <c r="F61" s="17" t="str">
+        <v>PSO+PSO</v>
+      </c>
+      <c r="G61" s="17" t="str">
+        <v>PSO+DE</v>
+      </c>
+      <c r="H61" s="17" t="str">
+        <v>PSO+FA</v>
+      </c>
+      <c r="I61" s="17" t="str">
+        <v>PSO+HS</v>
+      </c>
+      <c r="J61" s="17" t="str">
+        <v>PSO+RO</v>
+      </c>
+      <c r="K61" s="17" t="str">
+        <v>PSO+SO</v>
+      </c>
+      <c r="L61" s="17" t="str">
+        <v>PSO+CS</v>
+      </c>
+      <c r="M61" s="17" t="str">
+        <v>PSO+TS</v>
+      </c>
+      <c r="N61" s="17" t="str">
+        <v>PSO+MPSO</v>
+      </c>
+    </row>
+    <row r="62" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="E62" s="17" t="str">
+        <v>DE+GA</v>
+      </c>
+      <c r="F62" s="17" t="str">
+        <v>DE+PSO</v>
+      </c>
+      <c r="G62" s="17" t="str">
+        <v>DE+DE</v>
+      </c>
+      <c r="H62" s="17" t="str">
+        <v>DE+FA</v>
+      </c>
+      <c r="I62" s="17" t="str">
+        <v>DE+HS</v>
+      </c>
+      <c r="J62" s="17" t="str">
+        <v>DE+RO</v>
+      </c>
+      <c r="K62" s="17" t="str">
+        <v>DE+SO</v>
+      </c>
+      <c r="L62" s="17" t="str">
+        <v>DE+CS</v>
+      </c>
+      <c r="M62" s="17" t="str">
+        <v>DE+TS</v>
+      </c>
+      <c r="N62" s="17" t="str">
+        <v>DE+MPSO</v>
+      </c>
+    </row>
+    <row r="63" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="E63" s="17" t="str">
+        <v>FA+GA</v>
+      </c>
+      <c r="F63" s="17" t="str">
+        <v>FA+PSO</v>
+      </c>
+      <c r="G63" s="17" t="str">
+        <v>FA+DE</v>
+      </c>
+      <c r="H63" s="17" t="str">
+        <v>FA+FA</v>
+      </c>
+      <c r="I63" s="17" t="str">
+        <v>FA+HS</v>
+      </c>
+      <c r="J63" s="17" t="str">
+        <v>FA+RO</v>
+      </c>
+      <c r="K63" s="17" t="str">
+        <v>FA+SO</v>
+      </c>
+      <c r="L63" s="17" t="str">
+        <v>FA+CS</v>
+      </c>
+      <c r="M63" s="17" t="str">
+        <v>FA+TS</v>
+      </c>
+      <c r="N63" s="17" t="str">
+        <v>FA+MPSO</v>
+      </c>
+    </row>
+    <row r="64" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="E64" s="17" t="str">
+        <v>HS+GA</v>
+      </c>
+      <c r="F64" s="17" t="str">
+        <v>HS+PSO</v>
+      </c>
+      <c r="G64" s="17" t="str">
+        <v>HS+DE</v>
+      </c>
+      <c r="H64" s="17" t="str">
+        <v>HS+FA</v>
+      </c>
+      <c r="I64" s="17" t="str">
+        <v>HS+HS</v>
+      </c>
+      <c r="J64" s="17" t="str">
+        <v>HS+RO</v>
+      </c>
+      <c r="K64" s="17" t="str">
+        <v>HS+SO</v>
+      </c>
+      <c r="L64" s="17" t="str">
+        <v>HS+CS</v>
+      </c>
+      <c r="M64" s="17" t="str">
+        <v>HS+TS</v>
+      </c>
+      <c r="N64" s="17" t="str">
+        <v>HS+MPSO</v>
+      </c>
+    </row>
+    <row r="65" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E65" s="17" t="str">
+        <v>RO+GA</v>
+      </c>
+      <c r="F65" s="17" t="str">
+        <v>RO+PSO</v>
+      </c>
+      <c r="G65" s="17" t="str">
+        <v>RO+DE</v>
+      </c>
+      <c r="H65" s="17" t="str">
+        <v>RO+FA</v>
+      </c>
+      <c r="I65" s="17" t="str">
+        <v>RO+HS</v>
+      </c>
+      <c r="J65" s="17" t="str">
+        <v>RO+RO</v>
+      </c>
+      <c r="K65" s="17" t="str">
+        <v>RO+SO</v>
+      </c>
+      <c r="L65" s="17" t="str">
+        <v>RO+CS</v>
+      </c>
+      <c r="M65" s="17" t="str">
+        <v>RO+TS</v>
+      </c>
+      <c r="N65" s="17" t="str">
+        <v>RO+MPSO</v>
+      </c>
+    </row>
+    <row r="66" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E66" s="17" t="str">
+        <v>SO+GA</v>
+      </c>
+      <c r="F66" s="17" t="str">
+        <v>SO+PSO</v>
+      </c>
+      <c r="G66" s="17" t="str">
+        <v>SO+DE</v>
+      </c>
+      <c r="H66" s="17" t="str">
+        <v>SO+FA</v>
+      </c>
+      <c r="I66" s="17" t="str">
+        <v>SO+HS</v>
+      </c>
+      <c r="J66" s="17" t="str">
+        <v>SO+RO</v>
+      </c>
+      <c r="K66" s="17" t="str">
+        <v>SO+SO</v>
+      </c>
+      <c r="L66" s="17" t="str">
+        <v>SO+CS</v>
+      </c>
+      <c r="M66" s="17" t="str">
+        <v>SO+TS</v>
+      </c>
+      <c r="N66" s="17" t="str">
+        <v>SO+MPSO</v>
+      </c>
+    </row>
+    <row r="67" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E67" s="17" t="str">
+        <v>CS+GA</v>
+      </c>
+      <c r="F67" s="17" t="str">
+        <v>CS+PSO</v>
+      </c>
+      <c r="G67" s="17" t="str">
+        <v>CS+DE</v>
+      </c>
+      <c r="H67" s="17" t="str">
+        <v>CS+FA</v>
+      </c>
+      <c r="I67" s="17" t="str">
+        <v>CS+HS</v>
+      </c>
+      <c r="J67" s="17" t="str">
+        <v>CS+RO</v>
+      </c>
+      <c r="K67" s="17" t="str">
+        <v>CS+SO</v>
+      </c>
+      <c r="L67" s="17" t="str">
+        <v>CS+CS</v>
+      </c>
+      <c r="M67" s="17" t="str">
+        <v>CS+TS</v>
+      </c>
+      <c r="N67" s="17" t="str">
+        <v>CS+MPSO</v>
+      </c>
+    </row>
+    <row r="68" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E68" s="17" t="str">
+        <v>TS+GA</v>
+      </c>
+      <c r="F68" s="17" t="str">
+        <v>TS+PSO</v>
+      </c>
+      <c r="G68" s="17" t="str">
+        <v>TS+DE</v>
+      </c>
+      <c r="H68" s="17" t="str">
+        <v>TS+FA</v>
+      </c>
+      <c r="I68" s="17" t="str">
+        <v>TS+HS</v>
+      </c>
+      <c r="J68" s="17" t="str">
+        <v>TS+RO</v>
+      </c>
+      <c r="K68" s="17" t="str">
+        <v>TS+SO</v>
+      </c>
+      <c r="L68" s="17" t="str">
+        <v>TS+CS</v>
+      </c>
+      <c r="M68" s="17" t="str">
+        <v>TS+TS</v>
+      </c>
+      <c r="N68" s="17" t="str">
+        <v>TS+MPSO</v>
+      </c>
+    </row>
+    <row r="69" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E69" s="17" t="str">
+        <v>MPSO+GA</v>
+      </c>
+      <c r="F69" s="17" t="str">
+        <v>MPSO+PSO</v>
+      </c>
+      <c r="G69" s="17" t="str">
+        <v>MPSO+DE</v>
+      </c>
+      <c r="H69" s="17" t="str">
+        <v>MPSO+FA</v>
+      </c>
+      <c r="I69" s="17" t="str">
+        <v>MPSO+HS</v>
+      </c>
+      <c r="J69" s="17" t="str">
+        <v>MPSO+RO</v>
+      </c>
+      <c r="K69" s="17" t="str">
+        <v>MPSO+SO</v>
+      </c>
+      <c r="L69" s="17" t="str">
+        <v>MPSO+CS</v>
+      </c>
+      <c r="M69" s="17" t="str">
+        <v>MPSO+TS</v>
+      </c>
+      <c r="N69" s="17" t="str">
+        <v>MPSO+MPSO</v>
+      </c>
+    </row>
+    <row r="72" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E72" s="17" t="str" cm="1">
+        <f t="array" ref="E72:N81">_xlfn.ANCHORARRAY(F39)&amp;"+"&amp;_xlfn.ANCHORARRAY(E40)</f>
+        <v>GA+GA</v>
+      </c>
+      <c r="F72" s="17" t="str">
+        <v>PSO+GA</v>
+      </c>
+      <c r="G72" s="17" t="str">
+        <v>DE+GA</v>
+      </c>
+      <c r="H72" s="17" t="str">
+        <v>FA+GA</v>
+      </c>
+      <c r="I72" s="17" t="str">
+        <v>HS+GA</v>
+      </c>
+      <c r="J72" s="17" t="str">
+        <v>RO+GA</v>
+      </c>
+      <c r="K72" s="17" t="str">
+        <v>SO+GA</v>
+      </c>
+      <c r="L72" s="17" t="str">
+        <v>CS+GA</v>
+      </c>
+      <c r="M72" s="17" t="str">
+        <v>TS+GA</v>
+      </c>
+      <c r="N72" s="17" t="str">
+        <v>MPSO+GA</v>
+      </c>
+    </row>
+    <row r="73" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E73" s="17" t="str">
+        <v>GA+PSO</v>
+      </c>
+      <c r="F73" s="17" t="str">
+        <v>PSO+PSO</v>
+      </c>
+      <c r="G73" s="17" t="str">
+        <v>DE+PSO</v>
+      </c>
+      <c r="H73" s="17" t="str">
+        <v>FA+PSO</v>
+      </c>
+      <c r="I73" s="17" t="str">
+        <v>HS+PSO</v>
+      </c>
+      <c r="J73" s="17" t="str">
+        <v>RO+PSO</v>
+      </c>
+      <c r="K73" s="17" t="str">
+        <v>SO+PSO</v>
+      </c>
+      <c r="L73" s="17" t="str">
+        <v>CS+PSO</v>
+      </c>
+      <c r="M73" s="17" t="str">
+        <v>TS+PSO</v>
+      </c>
+      <c r="N73" s="17" t="str">
+        <v>MPSO+PSO</v>
+      </c>
+    </row>
+    <row r="74" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E74" s="17" t="str">
+        <v>GA+DE</v>
+      </c>
+      <c r="F74" s="17" t="str">
+        <v>PSO+DE</v>
+      </c>
+      <c r="G74" s="17" t="str">
+        <v>DE+DE</v>
+      </c>
+      <c r="H74" s="17" t="str">
+        <v>FA+DE</v>
+      </c>
+      <c r="I74" s="17" t="str">
+        <v>HS+DE</v>
+      </c>
+      <c r="J74" s="17" t="str">
+        <v>RO+DE</v>
+      </c>
+      <c r="K74" s="17" t="str">
+        <v>SO+DE</v>
+      </c>
+      <c r="L74" s="17" t="str">
+        <v>CS+DE</v>
+      </c>
+      <c r="M74" s="17" t="str">
+        <v>TS+DE</v>
+      </c>
+      <c r="N74" s="17" t="str">
+        <v>MPSO+DE</v>
+      </c>
+    </row>
+    <row r="75" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E75" s="17" t="str">
+        <v>GA+FA</v>
+      </c>
+      <c r="F75" s="17" t="str">
+        <v>PSO+FA</v>
+      </c>
+      <c r="G75" s="17" t="str">
+        <v>DE+FA</v>
+      </c>
+      <c r="H75" s="17" t="str">
+        <v>FA+FA</v>
+      </c>
+      <c r="I75" s="17" t="str">
+        <v>HS+FA</v>
+      </c>
+      <c r="J75" s="17" t="str">
+        <v>RO+FA</v>
+      </c>
+      <c r="K75" s="17" t="str">
+        <v>SO+FA</v>
+      </c>
+      <c r="L75" s="17" t="str">
+        <v>CS+FA</v>
+      </c>
+      <c r="M75" s="17" t="str">
+        <v>TS+FA</v>
+      </c>
+      <c r="N75" s="17" t="str">
+        <v>MPSO+FA</v>
+      </c>
+    </row>
+    <row r="76" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E76" s="17" t="str">
+        <v>GA+HS</v>
+      </c>
+      <c r="F76" s="17" t="str">
+        <v>PSO+HS</v>
+      </c>
+      <c r="G76" s="17" t="str">
+        <v>DE+HS</v>
+      </c>
+      <c r="H76" s="17" t="str">
+        <v>FA+HS</v>
+      </c>
+      <c r="I76" s="17" t="str">
+        <v>HS+HS</v>
+      </c>
+      <c r="J76" s="17" t="str">
+        <v>RO+HS</v>
+      </c>
+      <c r="K76" s="17" t="str">
+        <v>SO+HS</v>
+      </c>
+      <c r="L76" s="17" t="str">
+        <v>CS+HS</v>
+      </c>
+      <c r="M76" s="17" t="str">
+        <v>TS+HS</v>
+      </c>
+      <c r="N76" s="17" t="str">
+        <v>MPSO+HS</v>
+      </c>
+    </row>
+    <row r="77" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E77" s="17" t="str">
+        <v>GA+RO</v>
+      </c>
+      <c r="F77" s="17" t="str">
+        <v>PSO+RO</v>
+      </c>
+      <c r="G77" s="17" t="str">
+        <v>DE+RO</v>
+      </c>
+      <c r="H77" s="17" t="str">
+        <v>FA+RO</v>
+      </c>
+      <c r="I77" s="17" t="str">
+        <v>HS+RO</v>
+      </c>
+      <c r="J77" s="17" t="str">
+        <v>RO+RO</v>
+      </c>
+      <c r="K77" s="17" t="str">
+        <v>SO+RO</v>
+      </c>
+      <c r="L77" s="17" t="str">
+        <v>CS+RO</v>
+      </c>
+      <c r="M77" s="17" t="str">
+        <v>TS+RO</v>
+      </c>
+      <c r="N77" s="17" t="str">
+        <v>MPSO+RO</v>
+      </c>
+    </row>
+    <row r="78" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E78" s="17" t="str">
+        <v>GA+SO</v>
+      </c>
+      <c r="F78" s="17" t="str">
+        <v>PSO+SO</v>
+      </c>
+      <c r="G78" s="17" t="str">
+        <v>DE+SO</v>
+      </c>
+      <c r="H78" s="17" t="str">
+        <v>FA+SO</v>
+      </c>
+      <c r="I78" s="17" t="str">
+        <v>HS+SO</v>
+      </c>
+      <c r="J78" s="17" t="str">
+        <v>RO+SO</v>
+      </c>
+      <c r="K78" s="17" t="str">
+        <v>SO+SO</v>
+      </c>
+      <c r="L78" s="17" t="str">
+        <v>CS+SO</v>
+      </c>
+      <c r="M78" s="17" t="str">
+        <v>TS+SO</v>
+      </c>
+      <c r="N78" s="17" t="str">
+        <v>MPSO+SO</v>
+      </c>
+    </row>
+    <row r="79" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E79" s="17" t="str">
+        <v>GA+CS</v>
+      </c>
+      <c r="F79" s="17" t="str">
+        <v>PSO+CS</v>
+      </c>
+      <c r="G79" s="17" t="str">
+        <v>DE+CS</v>
+      </c>
+      <c r="H79" s="17" t="str">
+        <v>FA+CS</v>
+      </c>
+      <c r="I79" s="17" t="str">
+        <v>HS+CS</v>
+      </c>
+      <c r="J79" s="17" t="str">
+        <v>RO+CS</v>
+      </c>
+      <c r="K79" s="17" t="str">
+        <v>SO+CS</v>
+      </c>
+      <c r="L79" s="17" t="str">
+        <v>CS+CS</v>
+      </c>
+      <c r="M79" s="17" t="str">
+        <v>TS+CS</v>
+      </c>
+      <c r="N79" s="17" t="str">
+        <v>MPSO+CS</v>
+      </c>
+    </row>
+    <row r="80" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E80" s="17" t="str">
+        <v>GA+TS</v>
+      </c>
+      <c r="F80" s="17" t="str">
+        <v>PSO+TS</v>
+      </c>
+      <c r="G80" s="17" t="str">
+        <v>DE+TS</v>
+      </c>
+      <c r="H80" s="17" t="str">
+        <v>FA+TS</v>
+      </c>
+      <c r="I80" s="17" t="str">
+        <v>HS+TS</v>
+      </c>
+      <c r="J80" s="17" t="str">
+        <v>RO+TS</v>
+      </c>
+      <c r="K80" s="17" t="str">
+        <v>SO+TS</v>
+      </c>
+      <c r="L80" s="17" t="str">
+        <v>CS+TS</v>
+      </c>
+      <c r="M80" s="17" t="str">
+        <v>TS+TS</v>
+      </c>
+      <c r="N80" s="17" t="str">
+        <v>MPSO+TS</v>
+      </c>
+    </row>
+    <row r="81" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E81" s="17" t="str">
+        <v>GA+MPSO</v>
+      </c>
+      <c r="F81" s="17" t="str">
+        <v>PSO+MPSO</v>
+      </c>
+      <c r="G81" s="17" t="str">
+        <v>DE+MPSO</v>
+      </c>
+      <c r="H81" s="17" t="str">
+        <v>FA+MPSO</v>
+      </c>
+      <c r="I81" s="17" t="str">
+        <v>HS+MPSO</v>
+      </c>
+      <c r="J81" s="17" t="str">
+        <v>RO+MPSO</v>
+      </c>
+      <c r="K81" s="17" t="str">
+        <v>SO+MPSO</v>
+      </c>
+      <c r="L81" s="17" t="str">
+        <v>CS+MPSO</v>
+      </c>
+      <c r="M81" s="17" t="str">
+        <v>TS+MPSO</v>
+      </c>
+      <c r="N81" s="17" t="str">
+        <v>MPSO+MPSO</v>
+      </c>
+    </row>
+    <row r="84" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E84" s="17" cm="1">
+        <f t="array" ref="E84:N93">_xlfn.MAP(_xlfn.ANCHORARRAY(E60),_xlfn.ANCHORARRAY(E72),_xlfn.LAMBDA(_xlpm.x,_xlpm.y,SUM((_a=_xlpm.x)+(_a=_xlpm.y))))</f>
+        <v>0</v>
+      </c>
+      <c r="F84" s="17">
+        <v>6</v>
+      </c>
+      <c r="G84" s="17">
+        <v>0</v>
+      </c>
+      <c r="H84" s="17">
+        <v>0</v>
+      </c>
+      <c r="I84" s="17">
+        <v>0</v>
+      </c>
+      <c r="J84" s="17">
+        <v>1</v>
+      </c>
+      <c r="K84" s="17">
+        <v>1</v>
+      </c>
+      <c r="L84" s="17">
+        <v>1</v>
+      </c>
+      <c r="M84" s="17">
+        <v>1</v>
+      </c>
+      <c r="N84" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E85" s="17">
+        <v>6</v>
+      </c>
+      <c r="F85" s="17">
+        <v>0</v>
+      </c>
+      <c r="G85" s="17">
+        <v>1</v>
+      </c>
+      <c r="H85" s="17">
+        <v>0</v>
+      </c>
+      <c r="I85" s="17">
+        <v>2</v>
+      </c>
+      <c r="J85" s="17">
+        <v>0</v>
+      </c>
+      <c r="K85" s="17">
+        <v>1</v>
+      </c>
+      <c r="L85" s="17">
+        <v>0</v>
+      </c>
+      <c r="M85" s="17">
+        <v>0</v>
+      </c>
+      <c r="N85" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E86" s="17">
+        <v>0</v>
+      </c>
+      <c r="F86" s="17">
+        <v>1</v>
+      </c>
+      <c r="G86" s="17">
+        <v>0</v>
+      </c>
+      <c r="H86" s="17">
+        <v>0</v>
+      </c>
+      <c r="I86" s="17">
+        <v>0</v>
+      </c>
+      <c r="J86" s="17">
+        <v>0</v>
+      </c>
+      <c r="K86" s="17">
+        <v>0</v>
+      </c>
+      <c r="L86" s="17">
+        <v>0</v>
+      </c>
+      <c r="M86" s="17">
+        <v>0</v>
+      </c>
+      <c r="N86" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E87" s="17">
+        <v>0</v>
+      </c>
+      <c r="F87" s="17">
+        <v>0</v>
+      </c>
+      <c r="G87" s="17">
+        <v>0</v>
+      </c>
+      <c r="H87" s="17">
+        <v>0</v>
+      </c>
+      <c r="I87" s="17">
+        <v>1</v>
+      </c>
+      <c r="J87" s="17">
+        <v>0</v>
+      </c>
+      <c r="K87" s="17">
+        <v>0</v>
+      </c>
+      <c r="L87" s="17">
+        <v>0</v>
+      </c>
+      <c r="M87" s="17">
+        <v>0</v>
+      </c>
+      <c r="N87" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E88" s="17">
+        <v>0</v>
+      </c>
+      <c r="F88" s="17">
+        <v>2</v>
+      </c>
+      <c r="G88" s="17">
+        <v>0</v>
+      </c>
+      <c r="H88" s="17">
+        <v>1</v>
+      </c>
+      <c r="I88" s="17">
+        <v>0</v>
+      </c>
+      <c r="J88" s="17">
+        <v>0</v>
+      </c>
+      <c r="K88" s="17">
+        <v>2</v>
+      </c>
+      <c r="L88" s="17">
+        <v>0</v>
+      </c>
+      <c r="M88" s="17">
+        <v>0</v>
+      </c>
+      <c r="N88" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E89" s="17">
+        <v>1</v>
+      </c>
+      <c r="F89" s="17">
+        <v>0</v>
+      </c>
+      <c r="G89" s="17">
+        <v>0</v>
+      </c>
+      <c r="H89" s="17">
+        <v>0</v>
+      </c>
+      <c r="I89" s="17">
+        <v>0</v>
+      </c>
+      <c r="J89" s="17">
+        <v>0</v>
+      </c>
+      <c r="K89" s="17">
+        <v>0</v>
+      </c>
+      <c r="L89" s="17">
+        <v>0</v>
+      </c>
+      <c r="M89" s="17">
+        <v>0</v>
+      </c>
+      <c r="N89" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E90" s="17">
+        <v>1</v>
+      </c>
+      <c r="F90" s="17">
+        <v>1</v>
+      </c>
+      <c r="G90" s="17">
+        <v>0</v>
+      </c>
+      <c r="H90" s="17">
+        <v>0</v>
+      </c>
+      <c r="I90" s="17">
+        <v>2</v>
+      </c>
+      <c r="J90" s="17">
+        <v>0</v>
+      </c>
+      <c r="K90" s="17">
+        <v>0</v>
+      </c>
+      <c r="L90" s="17">
+        <v>0</v>
+      </c>
+      <c r="M90" s="17">
+        <v>1</v>
+      </c>
+      <c r="N90" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E91" s="17">
+        <v>1</v>
+      </c>
+      <c r="F91" s="17">
+        <v>0</v>
+      </c>
+      <c r="G91" s="17">
+        <v>0</v>
+      </c>
+      <c r="H91" s="17">
+        <v>0</v>
+      </c>
+      <c r="I91" s="17">
+        <v>0</v>
+      </c>
+      <c r="J91" s="17">
+        <v>0</v>
+      </c>
+      <c r="K91" s="17">
+        <v>0</v>
+      </c>
+      <c r="L91" s="17">
+        <v>0</v>
+      </c>
+      <c r="M91" s="17">
+        <v>0</v>
+      </c>
+      <c r="N91" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E92" s="17">
+        <v>1</v>
+      </c>
+      <c r="F92" s="17">
+        <v>0</v>
+      </c>
+      <c r="G92" s="17">
+        <v>0</v>
+      </c>
+      <c r="H92" s="17">
+        <v>0</v>
+      </c>
+      <c r="I92" s="17">
+        <v>0</v>
+      </c>
+      <c r="J92" s="17">
+        <v>0</v>
+      </c>
+      <c r="K92" s="17">
+        <v>1</v>
+      </c>
+      <c r="L92" s="17">
+        <v>0</v>
+      </c>
+      <c r="M92" s="17">
+        <v>0</v>
+      </c>
+      <c r="N92" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E93" s="17">
+        <v>0</v>
+      </c>
+      <c r="F93" s="17">
+        <v>0</v>
+      </c>
+      <c r="G93" s="17">
+        <v>0</v>
+      </c>
+      <c r="H93" s="17">
+        <v>0</v>
+      </c>
+      <c r="I93" s="17">
+        <v>1</v>
+      </c>
+      <c r="J93" s="17">
+        <v>0</v>
+      </c>
+      <c r="K93" s="17">
+        <v>0</v>
+      </c>
+      <c r="L93" s="17">
+        <v>0</v>
+      </c>
+      <c r="M93" s="17">
+        <v>0</v>
+      </c>
+      <c r="N93" s="17">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:O1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding issues with the problem
There are always definitional issues with these problems. This does not detract from how useful these are as a learning experience.
</commit_message>
<xml_diff>
--- a/CH-048 Transformation.xlsx
+++ b/CH-048 Transformation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{A3E24027-88E8-42B4-B0B4-486B39F25AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27C0D9DD-FA62-4E43-B5C1-12AB76A17290}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{A3E24027-88E8-42B4-B0B4-486B39F25AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{699C9EB5-504B-4989-BAFD-AEF140E2CDFB}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="30">
   <si>
     <t>FA+HS</t>
   </si>
@@ -151,12 +151,18 @@
   <si>
     <t>This is a wonderful solution.</t>
   </si>
+  <si>
+    <t>It appears that combinations like GA+GA are not valid. If you add GA+GA, it will record as 2.</t>
+  </si>
+  <si>
+    <t>Why does SO come through as lower case.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +196,13 @@
       <color theme="1"/>
       <name val="Aptos Mono"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF7030A0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -341,11 +354,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -410,12 +424,14 @@
     <xf numFmtId="3" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comment" xfId="2" xr:uid="{89D04BF6-262B-4446-B5CB-A7FE09B02692}"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -461,7 +477,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="3044446" y="2355849"/>
-          <a:ext cx="5794752" cy="2216150"/>
+          <a:ext cx="5794752" cy="2339975"/>
           <a:chOff x="4119814" y="1849363"/>
           <a:chExt cx="4569974" cy="2393950"/>
         </a:xfrm>
@@ -1057,19 +1073,19 @@
       <c r="B1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
@@ -1582,19 +1598,19 @@
       <c r="B1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
     </row>
     <row r="2" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
@@ -3255,7 +3271,7 @@
   <dimension ref="A1:AA93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3266,25 +3282,25 @@
     <col min="6" max="15" width="4.09765625" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-    </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+    </row>
+    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="8" t="s">
         <v>19</v>
@@ -3321,7 +3337,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="8" t="s">
         <v>1</v>
@@ -3350,8 +3366,11 @@
         <v>1</v>
       </c>
       <c r="O3" s="14"/>
-    </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="Q3" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="7" t="s">
         <v>14</v>
@@ -3379,7 +3398,7 @@
       <c r="N4" s="13"/>
       <c r="O4" s="14"/>
     </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="8" t="s">
         <v>18</v>
@@ -3401,7 +3420,7 @@
       <c r="N5" s="13"/>
       <c r="O5" s="14"/>
     </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="20" t="s">
         <v>0</v>
@@ -3422,7 +3441,7 @@
       <c r="N6" s="13"/>
       <c r="O6" s="14"/>
     </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="7" t="s">
         <v>1</v>
@@ -3450,7 +3469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="7" t="s">
         <v>2</v>
@@ -3470,8 +3489,11 @@
       <c r="M8" s="13"/>
       <c r="N8" s="13"/>
       <c r="O8" s="14"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q8" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="7" t="s">
         <v>16</v>
@@ -3500,7 +3522,7 @@
       </c>
       <c r="O9" s="16"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="8" t="s">
         <v>3</v>
@@ -3522,7 +3544,7 @@
       <c r="N10" s="15"/>
       <c r="O10" s="16"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="22" t="s">
         <v>21</v>
@@ -3546,7 +3568,7 @@
       <c r="N11" s="15"/>
       <c r="O11" s="16"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
@@ -3569,7 +3591,7 @@
       <c r="N12" s="15"/>
       <c r="O12" s="16"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="8" t="s">
         <v>4</v>
@@ -3587,21 +3609,21 @@
       <c r="N13"/>
       <c r="O13"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="8" t="s">
         <v>22</v>
@@ -3648,7 +3670,7 @@
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
       <c r="H21" s="18"/>
-      <c r="P21" s="25" t="s">
+      <c r="P21" s="24" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>